<commit_message>
Enhance schedule data saving: Update save_schedule_data endpoint to handle empty schedules, ensure correct data types, and improve error handling. Update frontend alert messages for better user feedback.
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,13 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -460,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>example_audio_1.mp3</t>
+          <t>1_Brahme Muhurte.mp3</t>
         </is>
       </c>
       <c r="D2" t="b">

</xml_diff>